<commit_message>
updated Excel with missing AUC
</commit_message>
<xml_diff>
--- a/CM_results_Angie_7_datasets_One_Table.xlsx
+++ b/CM_results_Angie_7_datasets_One_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/az/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/az/Documents/GitHub/Spring_2019_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A69F542-0EBE-7649-A07E-1B2AFF55EA73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4311A8A0-485A-0C4D-88BF-E07D8D975CB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28080" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All-in-one" sheetId="9" r:id="rId1"/>
@@ -360,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -588,13 +588,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -628,9 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -642,9 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -712,18 +769,6 @@
     <xf numFmtId="49" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -734,6 +779,54 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -822,6 +915,141 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>682160</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>37180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>682520</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>40780</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0DCE85-1120-3B48-80B2-DFEA5F309704}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2333160" y="1624680"/>
+            <a:ext cx="360" cy="3600"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0DCE85-1120-3B48-80B2-DFEA5F309704}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2324160" y="1615680"/>
+              <a:ext cx="18000" cy="21240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>736900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>126700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>737260</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127060</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32768A0F-C4A4-8E4C-90BA-F20FC2D8CB6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1562400" y="1180800"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32768A0F-C4A4-8E4C-90BA-F20FC2D8CB6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1553400" y="1172160"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -924,7 +1152,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1027,7 +1255,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1130,7 +1358,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1233,7 +1461,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1336,7 +1564,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1390,7 +1618,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1491,6 +1719,60 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-03-27T03:53:21.783"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'0'5'0,"0"-1"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-03-27T03:53:25.606"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'0'0'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2570,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606EB328-74EE-6745-8360-4136769218DF}">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2581,14 +2863,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="H2" s="41" t="s">
         <v>74</v>
       </c>
@@ -2609,34 +2891,34 @@
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="32"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="56" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="35" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="P3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="3" t="s">
@@ -2650,47 +2932,47 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <v>0.67549999999999999</v>
+      <c r="B4" s="5">
+        <v>0.67330000000000001</v>
       </c>
       <c r="C4" s="5">
-        <v>0.71079999999999999</v>
+        <v>0.72570000000000001</v>
       </c>
       <c r="D4" s="5">
-        <v>0.71579999999999999</v>
-      </c>
-      <c r="E4" s="32">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="E4" s="30">
         <v>0.71030000000000004</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="33"/>
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <v>0.62829999999999997</v>
       </c>
-      <c r="J4" s="21">
-        <v>0.68020000000000003</v>
-      </c>
-      <c r="K4" s="21">
+      <c r="J4" s="19">
+        <v>0.66690000000000005</v>
+      </c>
+      <c r="K4" s="19">
         <v>0.67179999999999995</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="24">
         <v>0.68089999999999995</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="16">
         <v>0.62719999999999998</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="19">
         <v>0.70579999999999998</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="19">
         <v>0.66180000000000005</v>
       </c>
-      <c r="R4" s="26">
+      <c r="R4" s="24">
         <v>0.68979999999999997</v>
       </c>
     </row>
@@ -2702,43 +2984,43 @@
         <v>0.80020000000000002</v>
       </c>
       <c r="C5" s="8">
-        <v>0.70530000000000004</v>
+        <v>0.70860000000000001</v>
       </c>
       <c r="D5" s="8">
-        <v>0.73950000000000005</v>
-      </c>
-      <c r="E5" s="33">
+        <v>0.69979999999999998</v>
+      </c>
+      <c r="E5" s="31">
         <v>0.71079999999999999</v>
       </c>
-      <c r="F5" s="36"/>
+      <c r="F5" s="34"/>
       <c r="H5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>0.74329999999999996</v>
       </c>
-      <c r="J5" s="18">
-        <v>0.62409999999999999</v>
-      </c>
-      <c r="K5" s="18">
+      <c r="J5" s="16">
+        <v>0.60870000000000002</v>
+      </c>
+      <c r="K5" s="16">
         <v>0.60170000000000001</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="17">
         <v>0.65780000000000005</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="16">
         <v>0.69489999999999996</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="16">
         <v>0.58430000000000004</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="16">
         <v>0.53259999999999996</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R5" s="17">
         <v>0.60189999999999999</v>
       </c>
     </row>
@@ -2747,46 +3029,46 @@
         <v>5</v>
       </c>
       <c r="B6" s="8">
-        <v>0.55079999999999996</v>
+        <v>0.5464</v>
       </c>
       <c r="C6" s="8">
-        <v>0.71630000000000005</v>
+        <v>0.74280000000000002</v>
       </c>
       <c r="D6" s="8">
-        <v>0.69210000000000005</v>
-      </c>
-      <c r="E6" s="33">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="E6" s="31">
         <v>0.7097</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>0.51329999999999998</v>
       </c>
-      <c r="J6" s="18">
-        <v>0.73629999999999995</v>
-      </c>
-      <c r="K6" s="18">
+      <c r="J6" s="16">
+        <v>0.72509999999999997</v>
+      </c>
+      <c r="K6" s="16">
         <v>0.7419</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="17">
         <v>0.70409999999999995</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="16">
         <v>0.5595</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="16">
         <v>0.82730000000000004</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="16">
         <v>0.79110000000000003</v>
       </c>
-      <c r="R6" s="19">
+      <c r="R6" s="17">
         <v>0.77769999999999995</v>
       </c>
     </row>
@@ -2795,46 +3077,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="8">
-        <v>0.71150000000000002</v>
+        <v>0.71009999999999995</v>
       </c>
       <c r="C7" s="8">
-        <v>0.70920000000000005</v>
+        <v>0.72089999999999999</v>
       </c>
       <c r="D7" s="8">
-        <v>0.72240000000000004</v>
-      </c>
-      <c r="E7" s="33">
+        <v>0.70440000000000003</v>
+      </c>
+      <c r="E7" s="31">
         <v>0.71040000000000003</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="H7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>0.66669999999999996</v>
       </c>
-      <c r="J7" s="18">
-        <v>0.66120000000000001</v>
-      </c>
-      <c r="K7" s="18">
+      <c r="J7" s="16">
+        <v>0.64529999999999998</v>
+      </c>
+      <c r="K7" s="16">
         <v>0.64710000000000001</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="17">
         <v>0.6734</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="16">
         <v>0.65080000000000005</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="16">
         <v>0.66510000000000002</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="16">
         <v>0.61160000000000003</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="17">
         <v>0.65990000000000004</v>
       </c>
     </row>
@@ -2843,46 +3125,46 @@
         <v>7</v>
       </c>
       <c r="B8" s="8">
-        <v>0.64049999999999996</v>
+        <v>0.63819999999999999</v>
       </c>
       <c r="C8" s="8">
-        <v>0.71319999999999995</v>
+        <v>0.73370000000000002</v>
       </c>
       <c r="D8" s="8">
-        <v>0.70599999999999996</v>
-      </c>
-      <c r="E8" s="33">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="E8" s="31">
         <v>0.71</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <v>0.60429999999999995</v>
       </c>
-      <c r="J8" s="18">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="K8" s="18">
+      <c r="J8" s="16">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="K8" s="16">
         <v>0.69979999999999998</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="17">
         <v>0.68969999999999998</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="16">
         <v>0.61199999999999999</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="16">
         <v>0.77190000000000003</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="16">
         <v>0.71830000000000005</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="17">
         <v>0.73019999999999996</v>
       </c>
     </row>
@@ -2894,43 +3176,43 @@
         <v>0.80020000000000002</v>
       </c>
       <c r="C9" s="8">
-        <v>0.70530000000000004</v>
+        <v>0.70860000000000001</v>
       </c>
       <c r="D9" s="8">
-        <v>0.73950000000000005</v>
-      </c>
-      <c r="E9" s="33">
+        <v>0.69979999999999998</v>
+      </c>
+      <c r="E9" s="31">
         <v>0.71079999999999999</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="H9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <v>0.74329999999999996</v>
       </c>
-      <c r="J9" s="18">
-        <v>0.62409999999999999</v>
-      </c>
-      <c r="K9" s="18">
+      <c r="J9" s="16">
+        <v>0.60870000000000002</v>
+      </c>
+      <c r="K9" s="16">
         <v>0.60170000000000001</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <v>0.65780000000000005</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="16">
         <v>0.69489999999999996</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="16">
         <v>0.58430000000000004</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="16">
         <v>0.53259999999999996</v>
       </c>
-      <c r="R9" s="19">
+      <c r="R9" s="17">
         <v>0.60189999999999999</v>
       </c>
     </row>
@@ -2938,39 +3220,54 @@
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="33">
+      <c r="B10" s="46">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="C10" s="46">
+        <v>0.81110000000000004</v>
+      </c>
+      <c r="D10" s="46">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="E10" s="31">
         <v>0.79190000000000005</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="H10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="21">
         <v>0.70169999999999999</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="19">
+      <c r="J10" s="47">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="K10" s="47">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="L10" s="17">
         <v>0.73629999999999995</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="21">
         <v>0.69899999999999995</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="21">
         <v>0.77180000000000004</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="21">
         <v>0.72740000000000005</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="17">
         <v>0.75219999999999998</v>
       </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="41" t="s">
@@ -2993,10 +3290,10 @@
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -3006,7 +3303,7 @@
       <c r="I13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="35" t="s">
         <v>1</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -3015,16 +3312,16 @@
       <c r="L13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="43" t="s">
+      <c r="N13" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="P13" s="45" t="s">
+      <c r="P13" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="Q13" s="45" t="s">
+      <c r="Q13" s="39" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3032,73 +3329,73 @@
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>0.69620000000000004</v>
       </c>
-      <c r="C14" s="21">
-        <v>0.90380000000000005</v>
-      </c>
-      <c r="D14" s="21">
+      <c r="C14" s="19">
+        <v>0.90190000000000003</v>
+      </c>
+      <c r="D14" s="19">
         <v>0.90580000000000005</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="24">
         <v>0.86539999999999995</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="16">
         <v>0.63439999999999996</v>
       </c>
-      <c r="J14" s="21">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="K14" s="21">
+      <c r="J14" s="19">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="K14" s="19">
         <v>0.66769999999999996</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="24">
         <v>0.69940000000000002</v>
       </c>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46">
-        <v>7</v>
-      </c>
-      <c r="P14" s="46">
+      <c r="N14" s="40"/>
+      <c r="O14" s="40">
+        <v>6</v>
+      </c>
+      <c r="P14" s="40">
         <v>3</v>
       </c>
-      <c r="Q14" s="46">
-        <v>2</v>
+      <c r="Q14" s="40">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <v>0.90769999999999995</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="16">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="17">
         <v>0.8538</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="16">
         <v>0.75629999999999997</v>
       </c>
-      <c r="J15" s="18">
-        <v>0.64549999999999996</v>
-      </c>
-      <c r="K15" s="18">
+      <c r="J15" s="16">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="K15" s="16">
         <v>0.65880000000000005</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="17">
         <v>0.67059999999999997</v>
       </c>
     </row>
@@ -3106,159 +3403,163 @@
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <v>0.48459999999999998</v>
       </c>
-      <c r="C16" s="18">
-        <v>0.96540000000000004</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="C16" s="16">
+        <v>0.96150000000000002</v>
+      </c>
+      <c r="D16" s="16">
         <v>0.95</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="17">
         <v>0.87690000000000001</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="16">
         <v>0.51259999999999994</v>
       </c>
-      <c r="J16" s="18">
-        <v>0.77839999999999998</v>
-      </c>
-      <c r="K16" s="18">
+      <c r="J16" s="16">
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="K16" s="16">
         <v>0.67649999999999999</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="17">
         <v>0.72819999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>0.74919999999999998</v>
       </c>
-      <c r="C17" s="18">
-        <v>0.89749999999999996</v>
-      </c>
-      <c r="D17" s="18">
+      <c r="C17" s="16">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="D17" s="16">
         <v>0.90139999999999998</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="17">
         <v>0.86380000000000001</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <v>0.67410000000000003</v>
       </c>
-      <c r="J17" s="18">
-        <v>0.6915</v>
-      </c>
-      <c r="K17" s="18">
+      <c r="J17" s="16">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="K17" s="16">
         <v>0.66469999999999996</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="17">
         <v>0.6905</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>0.63780000000000003</v>
       </c>
-      <c r="C18" s="18">
-        <v>0.96050000000000002</v>
-      </c>
-      <c r="D18" s="18">
+      <c r="C18" s="16">
+        <v>0.95630000000000004</v>
+      </c>
+      <c r="D18" s="16">
         <v>0.94510000000000005</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="17">
         <v>0.874</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="16">
         <v>0.60809999999999997</v>
       </c>
-      <c r="J18" s="18">
-        <v>0.74450000000000005</v>
-      </c>
-      <c r="K18" s="18">
+      <c r="J18" s="16">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="K18" s="16">
         <v>0.67069999999999996</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="17">
         <v>0.71160000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>0.90769999999999995</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>0.8538</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="16">
         <v>0.75629999999999997</v>
       </c>
-      <c r="J19" s="18">
-        <v>0.64549999999999996</v>
-      </c>
-      <c r="K19" s="18">
+      <c r="J19" s="16">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="K19" s="16">
         <v>0.65880000000000005</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="17">
         <v>0.67059999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="21">
         <v>0.85299999999999998</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="23">
+      <c r="C20" s="47">
+        <v>0.95379999999999998</v>
+      </c>
+      <c r="D20" s="21">
         <v>0.95440000000000003</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="17">
         <v>0.92889999999999995</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="21">
         <v>0.72</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="23">
+      <c r="J20" s="47">
+        <v>0.79590000000000005</v>
+      </c>
+      <c r="K20" s="21">
         <v>0.74750000000000005</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="17">
         <v>0.76119999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="41" t="s">
         <v>73</v>
       </c>
@@ -3274,12 +3575,12 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:12" ht="42" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="42" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -3292,235 +3593,238 @@
       <c r="I23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="37" t="s">
+      <c r="J23" s="35" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="35" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="O23" s="45"/>
+    </row>
+    <row r="24" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="16">
         <v>0.65090000000000003</v>
       </c>
-      <c r="C24" s="21">
-        <v>0.71479999999999999</v>
-      </c>
-      <c r="D24" s="21">
+      <c r="C24" s="19">
+        <v>0.70979999999999999</v>
+      </c>
+      <c r="D24" s="19">
         <v>0.68389999999999995</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="24">
         <v>0.69320000000000004</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="25">
         <v>0.69420000000000004</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="26">
         <v>0.75260000000000005</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="26">
         <v>0.73880000000000001</v>
       </c>
-      <c r="L24" s="28">
+      <c r="L24" s="26">
         <v>0.75070000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="16">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C25" s="18">
-        <v>0.67390000000000005</v>
-      </c>
-      <c r="D25" s="18">
+      <c r="C25" s="16">
+        <v>0.67820000000000003</v>
+      </c>
+      <c r="D25" s="16">
         <v>0.65800000000000003</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="17">
         <v>0.68820000000000003</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="25">
         <v>0.80049999999999999</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="25">
         <v>0.7087</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K25" s="25">
         <v>0.70599999999999996</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="25">
         <v>0.7651</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>0.52869999999999995</v>
       </c>
-      <c r="C26" s="18">
-        <v>0.75570000000000004</v>
-      </c>
-      <c r="D26" s="18">
+      <c r="C26" s="16">
+        <v>0.74139999999999995</v>
+      </c>
+      <c r="D26" s="16">
         <v>0.70979999999999999</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="17">
         <v>0.69830000000000003</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="25">
         <v>0.58789999999999998</v>
       </c>
-      <c r="J26" s="27">
+      <c r="J26" s="25">
         <v>0.79659999999999997</v>
       </c>
-      <c r="K26" s="27">
+      <c r="K26" s="25">
         <v>0.77170000000000005</v>
       </c>
-      <c r="L26" s="27">
+      <c r="L26" s="25">
         <v>0.73619999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>0.68889999999999996</v>
       </c>
-      <c r="C27" s="18">
-        <v>0.7026</v>
-      </c>
-      <c r="D27" s="18">
+      <c r="C27" s="16">
+        <v>0.70030000000000003</v>
+      </c>
+      <c r="D27" s="16">
         <v>0.67549999999999999</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="17">
         <v>0.69169999999999998</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="25">
         <v>0.72360000000000002</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="25">
         <v>0.74119999999999997</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K27" s="25">
         <v>0.73</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="25">
         <v>0.75419999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="16">
         <v>0.62119999999999997</v>
       </c>
-      <c r="C28" s="18">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="D28" s="18">
+      <c r="C28" s="16">
+        <v>0.72389999999999999</v>
+      </c>
+      <c r="D28" s="16">
         <v>0.69389999999999996</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="17">
         <v>0.69520000000000004</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="25">
         <v>0.66020000000000001</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="25">
         <v>0.77700000000000002</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="25">
         <v>0.75560000000000005</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="25">
         <v>0.74360000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="16">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C29" s="18">
-        <v>0.67390000000000005</v>
-      </c>
-      <c r="D29" s="18">
+      <c r="C29" s="16">
+        <v>0.67820000000000003</v>
+      </c>
+      <c r="D29" s="16">
         <v>0.65800000000000003</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="17">
         <v>0.68820000000000003</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="25">
         <v>0.80049999999999999</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J29" s="25">
         <v>0.7087</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="25">
         <v>0.70599999999999996</v>
       </c>
-      <c r="L29" s="27">
+      <c r="L29" s="25">
         <v>0.7651</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="21">
         <v>0.72570000000000001</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="23">
+      <c r="C30" s="47">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="D30" s="21">
         <v>0.75109999999999999</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="17">
         <v>0.76719999999999999</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="29">
+      <c r="I30" s="27">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="21">
         <v>0.84189999999999998</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30" s="27">
         <v>0.80910000000000004</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="25">
         <v>0.83179999999999998</v>
       </c>
     </row>
@@ -3535,6 +3839,7 @@
     <mergeCell ref="H12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3546,7 +3851,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3555,15 +3860,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -3586,7 +3891,7 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="54">
         <v>0.67549999999999999</v>
       </c>
       <c r="C3" s="5">
@@ -3595,7 +3900,7 @@
       <c r="D3" s="5">
         <v>0.71579999999999999</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="28">
         <v>0.71030000000000004</v>
       </c>
       <c r="F3" s="6"/>
@@ -3605,16 +3910,16 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="49">
         <v>0.80020000000000002</v>
       </c>
       <c r="C4" s="8">
         <v>0.70530000000000004</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="50">
         <v>0.73950000000000005</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>0.71079999999999999</v>
       </c>
       <c r="F4" s="10"/>
@@ -3630,10 +3935,10 @@
       <c r="C5" s="8">
         <v>0.71630000000000005</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="49">
         <v>0.69210000000000005</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <v>0.7097</v>
       </c>
       <c r="F5" s="10"/>
@@ -3652,7 +3957,7 @@
       <c r="D6" s="8">
         <v>0.72240000000000004</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="29">
         <v>0.71040000000000003</v>
       </c>
       <c r="F6" s="10"/>
@@ -3671,7 +3976,7 @@
       <c r="D7" s="8">
         <v>0.70599999999999996</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <v>0.71</v>
       </c>
       <c r="F7" s="10"/>
@@ -3690,7 +3995,7 @@
       <c r="D8" s="8">
         <v>0.73950000000000005</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="29">
         <v>0.71079999999999999</v>
       </c>
       <c r="F8" s="10"/>
@@ -3700,26 +4005,26 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="31">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="29">
         <v>0.79190000000000005</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="8"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3728,7 +4033,7 @@
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="8"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -3737,7 +4042,7 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="8"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3746,32 +4051,32 @@
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>57</v>
       </c>
       <c r="E16" s="9"/>
@@ -3779,12 +4084,12 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="9"/>
@@ -3792,33 +4097,33 @@
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>60</v>
       </c>
       <c r="E19" s="9"/>
@@ -3826,30 +4131,30 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="9"/>
@@ -3857,7 +4162,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -3866,7 +4171,7 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -3875,7 +4180,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -3884,8 +4189,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3922,15 +4227,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -3953,16 +4258,16 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.69620000000000004</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>0.90380000000000005</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <v>0.90580000000000005</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.86539999999999995</v>
       </c>
       <c r="F3" s="6"/>
@@ -3972,16 +4277,16 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>0.90769999999999995</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.8538</v>
       </c>
       <c r="F4" s="10"/>
@@ -3991,16 +4296,16 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>0.48459999999999998</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>0.96540000000000004</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.95</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>0.87690000000000001</v>
       </c>
       <c r="F5" s="10"/>
@@ -4010,16 +4315,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.74919999999999998</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.89749999999999996</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.90139999999999998</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.86380000000000001</v>
       </c>
       <c r="F6" s="10"/>
@@ -4029,16 +4334,16 @@
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>0.63780000000000003</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.96050000000000002</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>0.94510000000000005</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>0.874</v>
       </c>
       <c r="F7" s="10"/>
@@ -4048,16 +4353,16 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>0.90769999999999995</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>0.84230000000000005</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>0.8538</v>
       </c>
       <c r="F8" s="10"/>
@@ -4067,177 +4372,177 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>0.85299999999999998</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23">
+      <c r="C9" s="22"/>
+      <c r="D9" s="21">
         <v>0.95440000000000003</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>0.92889999999999995</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="19" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="25"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="22"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="22"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4246,7 +4551,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -4255,8 +4560,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4293,15 +4598,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -4324,16 +4629,16 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.65090000000000003</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>0.71479999999999999</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <v>0.68389999999999995</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.69320000000000004</v>
       </c>
       <c r="F3" s="6"/>
@@ -4343,16 +4648,16 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.67390000000000005</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.65800000000000003</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.68820000000000003</v>
       </c>
       <c r="F4" s="10"/>
@@ -4362,16 +4667,16 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>0.52869999999999995</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>0.75570000000000004</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.70979999999999999</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>0.69830000000000003</v>
       </c>
       <c r="F5" s="10"/>
@@ -4381,16 +4686,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.68889999999999996</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.7026</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.67549999999999999</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.69169999999999998</v>
       </c>
       <c r="F6" s="10"/>
@@ -4400,16 +4705,16 @@
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>0.62119999999999997</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.73399999999999999</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>0.69389999999999996</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>0.69520000000000004</v>
       </c>
       <c r="F7" s="10"/>
@@ -4419,16 +4724,16 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>0.67390000000000005</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.65800000000000003</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>0.68820000000000003</v>
       </c>
       <c r="F8" s="10"/>
@@ -4438,186 +4743,186 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>0.72570000000000001</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23">
+      <c r="C9" s="22"/>
+      <c r="D9" s="21">
         <v>0.75109999999999999</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>0.76719999999999999</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -4626,8 +4931,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4664,15 +4969,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -4695,16 +5000,16 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.62829999999999997</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>0.68020000000000003</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <v>0.67179999999999995</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.68089999999999995</v>
       </c>
       <c r="F3" s="6"/>
@@ -4714,16 +5019,16 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>0.74329999999999996</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.62409999999999999</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.60170000000000001</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.65780000000000005</v>
       </c>
       <c r="F4" s="10"/>
@@ -4733,16 +5038,16 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>0.51329999999999998</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>0.73629999999999995</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.7419</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>0.70409999999999995</v>
       </c>
       <c r="F5" s="10"/>
@@ -4752,16 +5057,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.66669999999999996</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.66120000000000001</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.64710000000000001</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.6734</v>
       </c>
       <c r="F6" s="10"/>
@@ -4771,16 +5076,16 @@
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>0.60429999999999995</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.70299999999999996</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>0.69979999999999998</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>0.68969999999999998</v>
       </c>
       <c r="F7" s="10"/>
@@ -4790,16 +5095,16 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>0.74329999999999996</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>0.62409999999999999</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.60170000000000001</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>0.65780000000000005</v>
       </c>
       <c r="F8" s="10"/>
@@ -4809,157 +5114,157 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>0.70169999999999999</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="19">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="17">
         <v>0.73629999999999995</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -4968,7 +5273,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -4977,7 +5282,7 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4986,7 +5291,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -4995,8 +5300,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5033,15 +5338,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5064,273 +5369,273 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.63439999999999996</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>0.71199999999999997</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <v>0.66769999999999996</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.69940000000000002</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>0.75629999999999997</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.64549999999999996</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.65880000000000005</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.67059999999999997</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>0.51259999999999994</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>0.77839999999999998</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.67649999999999999</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>0.72819999999999996</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.67410000000000003</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.6915</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.66469999999999996</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.6905</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>0.60809999999999997</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.74450000000000005</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>0.67069999999999996</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>0.71160000000000001</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>0.75629999999999997</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>0.64549999999999996</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.65880000000000005</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>0.67059999999999997</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>0.72</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23">
+      <c r="C9" s="22"/>
+      <c r="D9" s="21">
         <v>0.74750000000000005</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>0.76119999999999999</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="19"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="19"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="19"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -5339,7 +5644,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -5348,7 +5653,7 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -5357,7 +5662,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -5366,8 +5671,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5404,15 +5709,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5435,275 +5740,275 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="25">
         <v>0.69420000000000004</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>0.75260000000000005</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="26">
         <v>0.73880000000000001</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>0.75070000000000003</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="25">
         <v>0.80049999999999999</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="25">
         <v>0.7087</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <v>0.70599999999999996</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="25">
         <v>0.7651</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="25">
         <v>0.58789999999999998</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="25">
         <v>0.79659999999999997</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="25">
         <v>0.77170000000000005</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="25">
         <v>0.73619999999999997</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="25">
         <v>0.72360000000000002</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="25">
         <v>0.74119999999999997</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="25">
         <v>0.73</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>0.75419999999999998</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="25">
         <v>0.66020000000000001</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <v>0.77700000000000002</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <v>0.75560000000000005</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>0.74360000000000004</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="25">
         <v>0.80049999999999999</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="25">
         <v>0.7087</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <v>0.70599999999999996</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>0.7651</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="27">
         <v>0.78800000000000003</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="21">
         <v>0.84189999999999998</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="27">
         <v>0.80910000000000004</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>0.83179999999999998</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="19"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="19"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="19"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -5712,7 +6017,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -5721,7 +6026,7 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -5730,7 +6035,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -5739,8 +6044,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5777,15 +6082,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -5808,16 +6113,16 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>0.62719999999999998</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>0.70579999999999998</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <v>0.66180000000000005</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>0.68979999999999997</v>
       </c>
       <c r="F3" s="6"/>
@@ -5827,16 +6132,16 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>0.69489999999999996</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.58430000000000004</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.53259999999999996</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.60189999999999999</v>
       </c>
       <c r="F4" s="10"/>
@@ -5846,16 +6151,16 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>0.5595</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>0.82730000000000004</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.79110000000000003</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>0.77769999999999995</v>
       </c>
       <c r="F5" s="10"/>
@@ -5865,16 +6170,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.65080000000000005</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.66510000000000002</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.61160000000000003</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.65990000000000004</v>
       </c>
       <c r="F6" s="10"/>
@@ -5884,16 +6189,16 @@
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>0.61199999999999999</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.77190000000000003</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>0.71830000000000005</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>0.73019999999999996</v>
       </c>
       <c r="F7" s="10"/>
@@ -5903,16 +6208,16 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>0.69489999999999996</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>0.58430000000000004</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>0.53259999999999996</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>0.60189999999999999</v>
       </c>
       <c r="F8" s="10"/>
@@ -5922,161 +6227,161 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>0.69899999999999995</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="21">
         <v>0.77180000000000004</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <v>0.72740000000000005</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>0.75219999999999998</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="8"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -6085,7 +6390,7 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="8"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -6094,7 +6399,7 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="8"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -6103,7 +6408,7 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -6112,8 +6417,8 @@
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>

</xml_diff>